<commit_message>
new scaling tests results: LaMEM has now performed a simulation on 262’144 cores.
git-svn-id: svn+ssh://gaia.geo.uni-mainz.de/local/home/lkausb/svn/LaMEM/trunk@5515 26174531-3d5a-4d31-aba0-7a6658d032cb
</commit_message>
<xml_diff>
--- a/doc/ScalingTests/JUQUEEN/FallingBlock_Canonical/FallingBlock_Canonical_FDSTAG_CoupledMG/ScalingResultsSummary.xlsx
+++ b/doc/ScalingTests/JUQUEEN/FallingBlock_Canonical/FallingBlock_Canonical_FDSTAG_CoupledMG/ScalingResultsSummary.xlsx
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1078,7 +1078,7 @@
         <v>26</v>
       </c>
       <c r="H27">
-        <f>F27+G27</f>
+        <f t="shared" ref="H27:H40" si="3">F27+G27</f>
         <v>0</v>
       </c>
     </row>
@@ -1105,7 +1105,7 @@
         <v>113</v>
       </c>
       <c r="H28">
-        <f>F28+G28</f>
+        <f t="shared" si="3"/>
         <v>140.69999999999999</v>
       </c>
       <c r="I28">
@@ -1143,7 +1143,7 @@
         <v>60.3</v>
       </c>
       <c r="H29">
-        <f>F29+G29</f>
+        <f t="shared" si="3"/>
         <v>86.199999999999989</v>
       </c>
       <c r="I29">
@@ -1160,7 +1160,7 @@
     </row>
     <row r="30" spans="1:11">
       <c r="H30">
-        <f>F30+G30</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1169,7 +1169,7 @@
         <v>35</v>
       </c>
       <c r="H31">
-        <f>F31+G31</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1178,7 +1178,7 @@
         <v>25</v>
       </c>
       <c r="H32">
-        <f>F32+G32</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1205,18 +1205,18 @@
         <v>40.1</v>
       </c>
       <c r="H33">
-        <f>F33+G33</f>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="I33">
         <v>2.8E-3</v>
       </c>
       <c r="J33">
-        <f t="shared" ref="J33:J38" si="3">G33-I33</f>
+        <f t="shared" ref="J33:J40" si="4">G33-I33</f>
         <v>40.097200000000001</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" ref="K33:K38" si="4">J33/E33</f>
+        <f t="shared" ref="K33:K40" si="5">J33/E33</f>
         <v>2.8640857142857143</v>
       </c>
     </row>
@@ -1234,15 +1234,15 @@
         <v>11</v>
       </c>
       <c r="H34">
-        <f>F34+G34</f>
-        <v>0</v>
-      </c>
-      <c r="J34">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="J34">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="K34" s="2" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1269,18 +1269,18 @@
         <v>73.8</v>
       </c>
       <c r="H35">
-        <f>F35+G35</f>
+        <f t="shared" si="3"/>
         <v>112.6</v>
       </c>
       <c r="I35" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="J35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>73.795000000000002</v>
       </c>
       <c r="K35" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.8382692307692308</v>
       </c>
     </row>
@@ -1307,18 +1307,18 @@
         <v>75.599999999999994</v>
       </c>
       <c r="H36">
-        <f>F36+G36</f>
+        <f t="shared" si="3"/>
         <v>116.6</v>
       </c>
       <c r="I36" s="3">
         <v>8.3700000000000007E-3</v>
       </c>
       <c r="J36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>75.591629999999995</v>
       </c>
       <c r="K36" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.79969</v>
       </c>
     </row>
@@ -1345,18 +1345,18 @@
         <v>88.8</v>
       </c>
       <c r="H37">
-        <f>F37+G37</f>
+        <f t="shared" si="3"/>
         <v>132.69999999999999</v>
       </c>
       <c r="I37" s="3">
         <v>1.38E-2</v>
       </c>
       <c r="J37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>88.786199999999994</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.6904909090909088</v>
       </c>
     </row>
@@ -1383,18 +1383,18 @@
         <v>245.4</v>
       </c>
       <c r="H38">
-        <f>F38+G38</f>
+        <f t="shared" si="3"/>
         <v>309.8</v>
       </c>
       <c r="I38" s="3">
         <v>0.02</v>
       </c>
       <c r="J38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>245.38</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.7884090909090911</v>
       </c>
     </row>
@@ -1411,9 +1411,29 @@
       <c r="D39" t="s">
         <v>11</v>
       </c>
+      <c r="E39">
+        <v>118</v>
+      </c>
+      <c r="F39">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="G39">
+        <v>340.3</v>
+      </c>
       <c r="H39">
-        <f>F39+G39</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>415.20000000000005</v>
+      </c>
+      <c r="I39" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="4"/>
+        <v>340.28000000000003</v>
+      </c>
+      <c r="K39" s="2">
+        <f t="shared" si="5"/>
+        <v>2.8837288135593222</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -1429,9 +1449,29 @@
       <c r="D40" t="s">
         <v>11</v>
       </c>
+      <c r="E40">
+        <v>166</v>
+      </c>
+      <c r="F40">
+        <v>103.5</v>
+      </c>
+      <c r="G40">
+        <v>468.5</v>
+      </c>
       <c r="H40">
-        <f>F40+G40</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>572</v>
+      </c>
+      <c r="I40" s="3">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="4"/>
+        <v>468.45100000000002</v>
+      </c>
+      <c r="K40" s="2">
+        <f t="shared" si="5"/>
+        <v>2.8219939759036148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>